<commit_message>
Initial commit - National Hunt betting simulator
</commit_message>
<xml_diff>
--- a/Betting_Simulation/grouped_r_metrics.xlsx
+++ b/Betting_Simulation/grouped_r_metrics.xlsx
@@ -474,19 +474,19 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>14</v>
+        <v>46</v>
       </c>
       <c r="C2" t="n">
-        <v>11.33</v>
+        <v>4.030000000000001</v>
       </c>
       <c r="D2" t="n">
-        <v>17.33</v>
+        <v>39.03</v>
       </c>
       <c r="E2" t="n">
-        <v>-6</v>
+        <v>-35</v>
       </c>
       <c r="F2" t="n">
-        <v>57.1</v>
+        <v>23.9</v>
       </c>
     </row>
     <row r="3">
@@ -496,19 +496,19 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>5</v>
+        <v>42</v>
       </c>
       <c r="C3" t="n">
-        <v>8.5</v>
+        <v>23</v>
       </c>
       <c r="D3" t="n">
-        <v>11.5</v>
+        <v>56</v>
       </c>
       <c r="E3" t="n">
-        <v>-3</v>
+        <v>-33</v>
       </c>
       <c r="F3" t="n">
-        <v>40</v>
+        <v>21.4</v>
       </c>
     </row>
     <row r="4">
@@ -518,18 +518,20 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" t="inlineStr"/>
+        <v>-3</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -602,7 +604,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -649,19 +651,19 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="C2" t="n">
-        <v>-2</v>
+        <v>12.03</v>
       </c>
       <c r="D2" t="n">
-        <v>1</v>
+        <v>31.03</v>
       </c>
       <c r="E2" t="n">
-        <v>-3</v>
+        <v>-19</v>
       </c>
       <c r="F2" t="n">
-        <v>25</v>
+        <v>26.9</v>
       </c>
     </row>
     <row r="3">
@@ -671,19 +673,19 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="C3" t="n">
-        <v>21.83</v>
+        <v>2</v>
       </c>
       <c r="D3" t="n">
-        <v>27.83</v>
+        <v>25</v>
       </c>
       <c r="E3" t="n">
-        <v>-6</v>
+        <v>-23</v>
       </c>
       <c r="F3" t="n">
-        <v>60</v>
+        <v>17.9</v>
       </c>
     </row>
     <row r="4">
@@ -693,18 +695,20 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" t="inlineStr"/>
+        <v>-29</v>
+      </c>
+      <c r="F4" t="n">
+        <v>21.6</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -749,7 +753,7 @@
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>9–10</t>
+          <t>9</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -769,7 +773,7 @@
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>11–13</t>
+          <t>10</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -789,22 +793,42 @@
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
+          <t>11–13</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
           <t>14+</t>
         </is>
       </c>
-      <c r="B9" t="n">
-        <v>0</v>
-      </c>
-      <c r="C9" t="n">
-        <v>0</v>
-      </c>
-      <c r="D9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E9" t="n">
-        <v>0</v>
-      </c>
-      <c r="F9" t="inlineStr"/>
+      <c r="B10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -860,23 +884,23 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>SALISBURY</t>
+          <t>CATTERICK</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>19</v>
+        <v>91</v>
       </c>
       <c r="C2" t="n">
-        <v>19.83</v>
+        <v>24.03</v>
       </c>
       <c r="D2" t="n">
-        <v>28.83</v>
+        <v>95.03</v>
       </c>
       <c r="E2" t="n">
-        <v>-9</v>
+        <v>-71</v>
       </c>
       <c r="F2" t="n">
-        <v>52.6</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>